<commit_message>
LSUN included, wGAN-gp adjusts in the gradient penalty method
</commit_message>
<xml_diff>
--- a/Arch.xlsx
+++ b/Arch.xlsx
@@ -148,15 +148,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="992" min="1" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="992" min="1" style="1" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="1025" min="993" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -222,10 +222,10 @@
         <v>64</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>2</v>
@@ -376,14 +376,14 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="n">
         <f aca="false">ROUNDDOWN((B7+2*D7-(C7-1)-1)/E7+1,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="1" t="n">
@@ -403,32 +403,6 @@
         <f aca="false">(I7-1)*L7-2*K7+J7</f>
         <v>495</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0"/>
-      <c r="B8" s="1" t="n">
-        <f aca="false">F7</f>
-        <v>2</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <f aca="false">ROUNDDOWN((B8+2*D8-(C8-1)-1)/E8+1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="H8" s="0"/>
-      <c r="I8" s="0"/>
-      <c r="J8" s="0"/>
-      <c r="K8" s="0"/>
-      <c r="L8" s="0"/>
-      <c r="M8" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>